<commit_message>
hw7 update for normality part
</commit_message>
<xml_diff>
--- a/cs677/homework/HW7/Homework_7/PINS.xlsx
+++ b/cs677/homework/HW7/Homework_7/PINS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\BU学习\MET CS 677 A3\Homework_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1D3853DA-83D5-42CB-A56A-02546373D0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{06DD7169-2DF5-40A7-8073-A086C5CCA81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23040" windowHeight="11448" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PINS_Y1" sheetId="1" r:id="rId1"/>
@@ -6638,7 +6638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="A55" sqref="A55:F63"/>
     </sheetView>
   </sheetViews>
@@ -7884,7 +7884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>

</xml_diff>